<commit_message>
Finalised ABT Tag system.
</commit_message>
<xml_diff>
--- a/RPGOnline2/abt.xlsx
+++ b/RPGOnline2/abt.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="78">
   <si>
     <t>Format</t>
   </si>
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,12 +612,12 @@
     <col min="14" max="14" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -643,7 +643,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -671,7 +671,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>A3+1</f>
         <v>1</v>
@@ -704,19 +704,16 @@
         <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O4" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" ref="A5:A14" si="1">A4+1</f>
         <v>2</v>
@@ -755,7 +752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -796,7 +793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -833,7 +830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -874,7 +871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -915,7 +912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -957,7 +954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -996,7 +993,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1035,7 +1032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1077,7 +1074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1114,7 +1111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1749,13 +1746,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>